<commit_message>
Finished added class labels to excel, cleaned data
</commit_message>
<xml_diff>
--- a/spendingdata.xlsx
+++ b/spendingdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="1320" windowWidth="27700" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="440" windowWidth="37340" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="spendingdata.csv" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="399">
   <si>
     <t>Transaction Date</t>
   </si>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4101,7 +4101,7 @@
         <v>5542</v>
       </c>
       <c r="K70" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
         <v>5921</v>
       </c>
       <c r="K83" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -4767,6 +4767,9 @@
       <c r="J90">
         <v>5542</v>
       </c>
+      <c r="K90" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -4799,6 +4802,9 @@
       <c r="J91">
         <v>5812</v>
       </c>
+      <c r="K91" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -4831,6 +4837,9 @@
       <c r="J92">
         <v>5411</v>
       </c>
+      <c r="K92" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -4863,6 +4872,9 @@
       <c r="J93">
         <v>5699</v>
       </c>
+      <c r="K93" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -4895,6 +4907,9 @@
       <c r="J94">
         <v>5812</v>
       </c>
+      <c r="K94" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -4927,6 +4942,9 @@
       <c r="J95">
         <v>7999</v>
       </c>
+      <c r="K95" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -4959,8 +4977,11 @@
       <c r="J96">
         <v>5542</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>42756</v>
       </c>
@@ -4991,8 +5012,11 @@
       <c r="J97">
         <v>5912</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>42756</v>
       </c>
@@ -5023,8 +5047,11 @@
       <c r="J98">
         <v>5812</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>42756</v>
       </c>
@@ -5055,8 +5082,11 @@
       <c r="J99">
         <v>5812</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>42755</v>
       </c>
@@ -5087,8 +5117,11 @@
       <c r="J100">
         <v>5814</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>42755</v>
       </c>
@@ -5119,8 +5152,11 @@
       <c r="J101">
         <v>5812</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>42753</v>
       </c>
@@ -5151,8 +5187,11 @@
       <c r="J102">
         <v>5331</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>42752</v>
       </c>
@@ -5183,8 +5222,11 @@
       <c r="J103">
         <v>5812</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>42752</v>
       </c>
@@ -5215,8 +5257,11 @@
       <c r="J104">
         <v>5814</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>42752</v>
       </c>
@@ -5247,8 +5292,11 @@
       <c r="J105">
         <v>7538</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>42751</v>
       </c>
@@ -5279,8 +5327,11 @@
       <c r="J106">
         <v>5912</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K106" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>42750</v>
       </c>
@@ -5311,8 +5362,11 @@
       <c r="J107">
         <v>5912</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K107" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>42749</v>
       </c>
@@ -5343,8 +5397,11 @@
       <c r="J108">
         <v>5812</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K108" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>42748</v>
       </c>
@@ -5375,8 +5432,11 @@
       <c r="J109">
         <v>5411</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K109" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>42748</v>
       </c>
@@ -5407,8 +5467,11 @@
       <c r="J110">
         <v>5812</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K110" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>42747</v>
       </c>
@@ -5439,8 +5502,11 @@
       <c r="J111">
         <v>5812</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K111" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>42746</v>
       </c>
@@ -5471,8 +5537,11 @@
       <c r="J112">
         <v>7997</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K112" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>42745</v>
       </c>
@@ -5503,8 +5572,11 @@
       <c r="J113">
         <v>5942</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K113" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>42745</v>
       </c>
@@ -5535,8 +5607,11 @@
       <c r="J114">
         <v>5942</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K114" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>42745</v>
       </c>
@@ -5567,8 +5642,11 @@
       <c r="J115">
         <v>5812</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K115" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>42744</v>
       </c>
@@ -5599,8 +5677,11 @@
       <c r="J116">
         <v>5942</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K116" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>42744</v>
       </c>
@@ -5631,8 +5712,11 @@
       <c r="J117">
         <v>5965</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K117" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>42740</v>
       </c>
@@ -5663,8 +5747,11 @@
       <c r="J118">
         <v>5542</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K118" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>42732</v>
       </c>
@@ -5695,8 +5782,11 @@
       <c r="J119">
         <v>7299</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K119" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>42738</v>
       </c>
@@ -5721,8 +5811,11 @@
       <c r="J120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K120" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>42735</v>
       </c>
@@ -5753,8 +5846,11 @@
       <c r="J121">
         <v>5812</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K121" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>42735</v>
       </c>
@@ -5785,8 +5881,11 @@
       <c r="J122">
         <v>5812</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K122" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>42735</v>
       </c>
@@ -5817,8 +5916,11 @@
       <c r="J123">
         <v>5411</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K123" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>42734</v>
       </c>
@@ -5849,8 +5951,11 @@
       <c r="J124">
         <v>5732</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K124" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>42732</v>
       </c>
@@ -5881,8 +5986,11 @@
       <c r="J125">
         <v>4111</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K125" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>42732</v>
       </c>
@@ -5913,8 +6021,11 @@
       <c r="J126">
         <v>4111</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K126" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>42730</v>
       </c>
@@ -5945,8 +6056,11 @@
       <c r="J127">
         <v>5411</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K127" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>42730</v>
       </c>
@@ -5977,8 +6091,11 @@
       <c r="J128">
         <v>5941</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K128" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>42727</v>
       </c>
@@ -6009,8 +6126,11 @@
       <c r="J129">
         <v>5411</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K129" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>42725</v>
       </c>
@@ -6041,8 +6161,11 @@
       <c r="J130">
         <v>5411</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K130" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>42725</v>
       </c>
@@ -6073,8 +6196,11 @@
       <c r="J131">
         <v>5812</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K131" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>42725</v>
       </c>
@@ -6105,8 +6231,11 @@
       <c r="J132">
         <v>5941</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K132" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>42725</v>
       </c>
@@ -6137,8 +6266,11 @@
       <c r="J133">
         <v>5732</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K133" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>42725</v>
       </c>
@@ -6169,8 +6301,11 @@
       <c r="J134">
         <v>5735</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K134" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>42725</v>
       </c>
@@ -6201,8 +6336,11 @@
       <c r="J135">
         <v>5999</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K135" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>42724</v>
       </c>
@@ -6233,8 +6371,11 @@
       <c r="J136">
         <v>5812</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K136" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>42724</v>
       </c>
@@ -6265,8 +6406,11 @@
       <c r="J137">
         <v>5814</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K137" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>42723</v>
       </c>
@@ -6297,8 +6441,11 @@
       <c r="J138">
         <v>7933</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K138" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>42723</v>
       </c>
@@ -6329,8 +6476,11 @@
       <c r="J139">
         <v>7994</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K139" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>42723</v>
       </c>
@@ -6361,8 +6511,11 @@
       <c r="J140">
         <v>7994</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K140" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>42714</v>
       </c>
@@ -6393,8 +6546,11 @@
       <c r="J141">
         <v>5542</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K141" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>42709</v>
       </c>
@@ -6425,8 +6581,11 @@
       <c r="J142">
         <v>5814</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K142" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>42706</v>
       </c>
@@ -6451,8 +6610,11 @@
       <c r="J143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K143" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>42706</v>
       </c>
@@ -6474,8 +6636,11 @@
       <c r="J144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K144" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>42706</v>
       </c>
@@ -6497,8 +6662,11 @@
       <c r="J145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K145" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>42705</v>
       </c>
@@ -6520,8 +6688,11 @@
       <c r="J146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K146" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>42704</v>
       </c>
@@ -6552,8 +6723,11 @@
       <c r="J147">
         <v>5812</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K147" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>42703</v>
       </c>
@@ -6584,8 +6758,11 @@
       <c r="J148">
         <v>5814</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K148" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>42702</v>
       </c>
@@ -6616,8 +6793,11 @@
       <c r="J149">
         <v>7523</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K149" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>42701</v>
       </c>
@@ -6648,8 +6828,11 @@
       <c r="J150">
         <v>5411</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K150" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>42699</v>
       </c>
@@ -6680,8 +6863,11 @@
       <c r="J151">
         <v>5542</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K151" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>42697</v>
       </c>
@@ -6712,8 +6898,11 @@
       <c r="J152">
         <v>5812</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K152" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>42697</v>
       </c>
@@ -6744,8 +6933,11 @@
       <c r="J153">
         <v>7538</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K153" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>42696</v>
       </c>
@@ -6776,8 +6968,11 @@
       <c r="J154">
         <v>7523</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K154" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>42695</v>
       </c>
@@ -6808,8 +7003,11 @@
       <c r="J155">
         <v>5812</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K155" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>42695</v>
       </c>
@@ -6840,8 +7038,11 @@
       <c r="J156">
         <v>5812</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K156" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>42693</v>
       </c>
@@ -6872,8 +7073,11 @@
       <c r="J157">
         <v>5812</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K157" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>42693</v>
       </c>
@@ -6904,8 +7108,11 @@
       <c r="J158">
         <v>8641</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K158" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>42691</v>
       </c>
@@ -6936,8 +7143,11 @@
       <c r="J159">
         <v>7523</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K159" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>42691</v>
       </c>
@@ -6968,8 +7178,11 @@
       <c r="J160">
         <v>5812</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K160" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>42690</v>
       </c>
@@ -7000,8 +7213,11 @@
       <c r="J161">
         <v>7523</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K161" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>42689</v>
       </c>
@@ -7032,8 +7248,11 @@
       <c r="J162">
         <v>5814</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K162" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>42689</v>
       </c>
@@ -7064,8 +7283,11 @@
       <c r="J163">
         <v>5812</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K163" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>42688</v>
       </c>
@@ -7096,8 +7318,11 @@
       <c r="J164">
         <v>5542</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K164" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>42687</v>
       </c>
@@ -7128,8 +7353,11 @@
       <c r="J165">
         <v>5411</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K165" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>42686</v>
       </c>
@@ -7160,8 +7388,11 @@
       <c r="J166">
         <v>5812</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K166" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>42686</v>
       </c>
@@ -7192,8 +7423,11 @@
       <c r="J167">
         <v>7832</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K167" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>42686</v>
       </c>
@@ -7224,8 +7458,11 @@
       <c r="J168">
         <v>5812</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K168" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>42684</v>
       </c>
@@ -7256,8 +7493,11 @@
       <c r="J169">
         <v>7523</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K169" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>42684</v>
       </c>
@@ -7288,8 +7528,11 @@
       <c r="J170">
         <v>5814</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K170" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>42683</v>
       </c>
@@ -7320,8 +7563,11 @@
       <c r="J171">
         <v>5814</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K171" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>42683</v>
       </c>
@@ -7352,8 +7598,11 @@
       <c r="J172">
         <v>5814</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K172" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>42682</v>
       </c>
@@ -7384,8 +7633,11 @@
       <c r="J173">
         <v>5814</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K173" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>42682</v>
       </c>
@@ -7416,8 +7668,11 @@
       <c r="J174">
         <v>5814</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K174" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>42682</v>
       </c>
@@ -7448,8 +7703,11 @@
       <c r="J175">
         <v>7523</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K175" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>42679</v>
       </c>
@@ -7480,8 +7738,11 @@
       <c r="J176">
         <v>5814</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K176" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>42679</v>
       </c>
@@ -7512,8 +7773,11 @@
       <c r="J177">
         <v>5814</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K177" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>42679</v>
       </c>
@@ -7544,8 +7808,11 @@
       <c r="J178">
         <v>7523</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K178" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>42678</v>
       </c>
@@ -7576,8 +7843,11 @@
       <c r="J179">
         <v>5812</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K179" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>42678</v>
       </c>
@@ -7608,8 +7878,11 @@
       <c r="J180">
         <v>5812</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K180" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>42859</v>
       </c>
@@ -7631,8 +7904,11 @@
       <c r="J181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K181" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>42859</v>
       </c>
@@ -7654,8 +7930,11 @@
       <c r="J182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K182" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>42857</v>
       </c>
@@ -7680,8 +7959,11 @@
       <c r="J183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K183" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>42856</v>
       </c>
@@ -7703,8 +7985,11 @@
       <c r="J184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K184" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>42856</v>
       </c>
@@ -7735,8 +8020,11 @@
       <c r="J185">
         <v>5814</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K185" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>42855</v>
       </c>
@@ -7767,8 +8055,11 @@
       <c r="J186">
         <v>5310</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K186" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>42854</v>
       </c>
@@ -7799,8 +8090,11 @@
       <c r="J187">
         <v>5814</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K187" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>42854</v>
       </c>
@@ -7831,8 +8125,11 @@
       <c r="J188">
         <v>5912</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K188" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>42854</v>
       </c>
@@ -7863,8 +8160,11 @@
       <c r="J189">
         <v>5542</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K189" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>42853</v>
       </c>
@@ -7895,8 +8195,11 @@
       <c r="J190">
         <v>5814</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K190" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>42852</v>
       </c>
@@ -7927,8 +8230,11 @@
       <c r="J191">
         <v>5814</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K191" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>42851</v>
       </c>
@@ -7959,8 +8265,11 @@
       <c r="J192">
         <v>5814</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K192" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>42851</v>
       </c>
@@ -7991,8 +8300,11 @@
       <c r="J193">
         <v>5814</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K193" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>42850</v>
       </c>
@@ -8023,8 +8335,11 @@
       <c r="J194">
         <v>5814</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K194" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>42850</v>
       </c>
@@ -8055,8 +8370,11 @@
       <c r="J195">
         <v>7933</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K195" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>42850</v>
       </c>
@@ -8087,8 +8405,11 @@
       <c r="J196">
         <v>7933</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K196" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>42849</v>
       </c>
@@ -8119,8 +8440,11 @@
       <c r="J197">
         <v>5499</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K197" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>42849</v>
       </c>
@@ -8151,8 +8475,11 @@
       <c r="J198">
         <v>5812</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K198" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>42848</v>
       </c>
@@ -8183,8 +8510,11 @@
       <c r="J199">
         <v>5411</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K199" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>42846</v>
       </c>
@@ -8215,8 +8545,11 @@
       <c r="J200">
         <v>5812</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K200" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>42845</v>
       </c>
@@ -8247,8 +8580,11 @@
       <c r="J201">
         <v>5812</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K201" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>42845</v>
       </c>
@@ -8279,8 +8615,11 @@
       <c r="J202">
         <v>5542</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K202" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>42845</v>
       </c>
@@ -8311,8 +8650,11 @@
       <c r="J203">
         <v>5812</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K203" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>42845</v>
       </c>
@@ -8343,8 +8685,11 @@
       <c r="J204">
         <v>5814</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K204" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>42844</v>
       </c>
@@ -8375,8 +8720,11 @@
       <c r="J205">
         <v>5812</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K205" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>42843</v>
       </c>
@@ -8407,8 +8755,11 @@
       <c r="J206">
         <v>5814</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K206" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>42842</v>
       </c>
@@ -8439,8 +8790,11 @@
       <c r="J207">
         <v>5814</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K207" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>42841</v>
       </c>
@@ -8471,8 +8825,11 @@
       <c r="J208">
         <v>5812</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K208" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>42840</v>
       </c>
@@ -8503,8 +8860,11 @@
       <c r="J209">
         <v>5812</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K209" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>42839</v>
       </c>
@@ -8535,8 +8895,11 @@
       <c r="J210">
         <v>5651</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K210" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>42838</v>
       </c>
@@ -8567,8 +8930,11 @@
       <c r="J211">
         <v>5814</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K211" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>42837</v>
       </c>
@@ -8599,8 +8965,11 @@
       <c r="J212">
         <v>7922</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K212" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>42837</v>
       </c>
@@ -8631,8 +9000,11 @@
       <c r="J213">
         <v>5814</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K213" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>42836</v>
       </c>
@@ -8663,8 +9035,11 @@
       <c r="J214">
         <v>5812</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K214" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>42835</v>
       </c>
@@ -8695,8 +9070,11 @@
       <c r="J215">
         <v>5814</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K215" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>42835</v>
       </c>
@@ -8727,8 +9105,11 @@
       <c r="J216">
         <v>7832</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K216" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>42835</v>
       </c>
@@ -8759,8 +9140,11 @@
       <c r="J217">
         <v>5812</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K217" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>42834</v>
       </c>
@@ -8791,8 +9175,11 @@
       <c r="J218">
         <v>7832</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K218" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>42834</v>
       </c>
@@ -8823,8 +9210,11 @@
       <c r="J219">
         <v>5542</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K219" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>42834</v>
       </c>
@@ -8855,8 +9245,11 @@
       <c r="J220">
         <v>5912</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K220" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>42833</v>
       </c>
@@ -8887,8 +9280,11 @@
       <c r="J221">
         <v>5661</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K221" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>42833</v>
       </c>
@@ -8919,8 +9315,11 @@
       <c r="J222">
         <v>5499</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K222" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>42832</v>
       </c>
@@ -8951,8 +9350,11 @@
       <c r="J223">
         <v>5812</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K223" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>42831</v>
       </c>
@@ -8983,8 +9385,11 @@
       <c r="J224">
         <v>5814</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K224" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>42831</v>
       </c>
@@ -9015,8 +9420,11 @@
       <c r="J225">
         <v>5812</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K225" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>42831</v>
       </c>
@@ -9047,8 +9455,11 @@
       <c r="J226">
         <v>8042</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K226" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>42829</v>
       </c>
@@ -9078,6 +9489,9 @@
       </c>
       <c r="J227">
         <v>5814</v>
+      </c>
+      <c r="K227" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>